<commit_message>
Out of bounds time support
</commit_message>
<xml_diff>
--- a/scheds.xlsx
+++ b/scheds.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>07:00 AM</t>
   </si>
@@ -79,6 +79,12 @@
     <t>05:00 PM</t>
   </si>
   <si>
+    <t>05:30 PM</t>
+  </si>
+  <si>
+    <t>06:00 PM</t>
+  </si>
+  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -97,31 +103,34 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Modeling and Simulation</t>
+    <t>DATAMA2</t>
   </si>
   <si>
     <t>09:30 AM - 11:30 AM</t>
   </si>
   <si>
-    <t>Automata Theory</t>
+    <t>OPESYST</t>
   </si>
   <si>
     <t>01:00 PM - 03:00 PM</t>
   </si>
   <si>
-    <t>Physical Education 4</t>
-  </si>
-  <si>
-    <t>03:00 PM - 05:00 PM</t>
-  </si>
-  <si>
-    <t>Operating System</t>
-  </si>
-  <si>
-    <t>Database Management 2</t>
-  </si>
-  <si>
-    <t>Web Programming</t>
+    <t>MOBAPPL</t>
+  </si>
+  <si>
+    <t>07:30 AM - 09:30 AM</t>
+  </si>
+  <si>
+    <t>COMPAIS</t>
+  </si>
+  <si>
+    <t>WEBPROG</t>
+  </si>
+  <si>
+    <t>PEDUFOR</t>
+  </si>
+  <si>
+    <t>05:00 PM - 05:40 PM</t>
   </si>
 </sst>
 </file>
@@ -154,6 +163,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -173,12 +188,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:H25"/>
+  <dimension ref="B4:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -521,22 +530,22 @@
   <sheetData>
     <row r="4" spans="2:8">
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -548,78 +557,98 @@
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>33</v>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>28</v>
+      <c r="C12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="2" t="s">
@@ -635,109 +664,98 @@
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>34</v>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>30</v>
+      <c r="C19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>